<commit_message>
update datetime and verify analysis
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/9_Date_Time_Functions.xlsx
+++ b/2_Formulas_Functions/9_Date_Time_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B682AA-3284-4B67-84CE-D03F1625E05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E79171-D30D-4665-A15E-9C185E9A912F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18336" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="96">
   <si>
     <t>Email</t>
   </si>
@@ -585,7 +585,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Count</a:t>
+              <a:t>Count by Hour</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1885,25 +1885,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E7F13-C613-4452-9CDB-2C26D6876D9D}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.578125" customWidth="1"/>
+    <col min="2" max="2" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.26171875" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.20703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.9453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="14.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1928,8 +1931,45 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" s="16"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -1955,7 +1995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -1981,7 +2021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2007,7 +2047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -2033,7 +2073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -2059,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -2085,7 +2125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -2111,7 +2151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -2137,7 +2177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -2163,7 +2203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -2215,7 +2255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -2241,7 +2281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -2267,7 +2307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -2293,7 +2333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -2319,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -2345,7 +2385,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -2371,7 +2411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -2397,7 +2437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -2423,7 +2463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -2463,25 +2503,25 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83984375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="40" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.68359375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -2525,7 +2565,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -2568,14 +2608,14 @@
       </c>
       <c r="P2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45511</v>
+        <v>45538</v>
       </c>
       <c r="R2">
         <f ca="1">DATEDIF(D2,$P$2,"D")</f>
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -2618,10 +2658,10 @@
       </c>
       <c r="R3">
         <f ca="1">DATEDIF(D3,$P$2,"D")</f>
-        <v>456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2664,10 +2704,10 @@
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R21" ca="1" si="4">DATEDIF(D4,$P$2,"D")</f>
-        <v>383</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -2710,10 +2750,10 @@
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="4"/>
-        <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -2756,10 +2796,10 @@
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="4"/>
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -2802,10 +2842,10 @@
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="4"/>
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -2849,10 +2889,10 @@
       <c r="P8" s="9"/>
       <c r="R8">
         <f t="shared" ca="1" si="4"/>
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -2895,10 +2935,10 @@
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="4"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -2941,10 +2981,10 @@
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="4"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -2987,10 +3027,10 @@
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="4"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -3033,10 +3073,10 @@
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -3079,10 +3119,10 @@
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="4"/>
-        <v>560</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -3125,10 +3165,10 @@
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="4"/>
-        <v>509</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -3171,10 +3211,10 @@
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="4"/>
-        <v>433</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -3217,10 +3257,10 @@
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="4"/>
-        <v>343</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -3263,10 +3303,10 @@
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="4"/>
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -3309,10 +3349,10 @@
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="4"/>
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -3355,10 +3395,10 @@
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="4"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -3401,10 +3441,10 @@
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="4"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -3447,7 +3487,7 @@
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="4"/>
-        <v>89</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3459,25 +3499,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5E2CB8-8C8C-43FB-95B8-5A63A3C08A07}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -3522,7 +3562,7 @@
       </c>
       <c r="R1" s="16"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -3574,7 +3614,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -3627,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -3680,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -3733,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -3786,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -3839,7 +3879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -3892,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -3945,7 +3985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -3998,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -4051,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -4104,7 +4144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -4157,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -4210,7 +4250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -4263,7 +4303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -4316,7 +4356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -4369,7 +4409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -4422,7 +4462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -4475,7 +4515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -4528,7 +4568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -4581,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="Q22" s="14">
         <v>20</v>
       </c>
@@ -4590,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="Q23" s="14">
         <v>21</v>
       </c>
@@ -4599,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="Q24" s="14">
         <v>22</v>
       </c>
@@ -4608,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="Q25" s="14">
         <v>23</v>
       </c>
@@ -4617,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="Q26" s="14">
         <v>24</v>
       </c>

</xml_diff>